<commit_message>
ze finni for real
</commit_message>
<xml_diff>
--- a/Coefs.xlsx
+++ b/Coefs.xlsx
@@ -509,19 +509,19 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>3.152</v>
+        <v>3.154</v>
       </c>
       <c r="H2" t="n">
         <v>3.205</v>
       </c>
       <c r="I2" t="n">
-        <v>24.016</v>
+        <v>24.032</v>
       </c>
       <c r="J2" t="n">
-        <v>23.392</v>
+        <v>23.43</v>
       </c>
       <c r="K2" t="n">
-        <v>24.657</v>
+        <v>24.649</v>
       </c>
     </row>
     <row r="3">
@@ -578,10 +578,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.176</v>
+        <v>0.178</v>
       </c>
       <c r="E4" t="n">
-        <v>0.039</v>
+        <v>0.041</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -590,16 +590,16 @@
         <v>0.098</v>
       </c>
       <c r="H4" t="n">
-        <v>0.253</v>
+        <v>0.258</v>
       </c>
       <c r="I4" t="n">
-        <v>1.192</v>
+        <v>1.195</v>
       </c>
       <c r="J4" t="n">
         <v>1.103</v>
       </c>
       <c r="K4" t="n">
-        <v>1.288</v>
+        <v>1.295</v>
       </c>
     </row>
     <row r="5">
@@ -656,28 +656,28 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-0.109</v>
+        <v>-0.046</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04</v>
+        <v>0.045</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0069</v>
+        <v>0.3025</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.189</v>
+        <v>-0.134</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.03</v>
+        <v>0.042</v>
       </c>
       <c r="I6" t="n">
-        <v>0.896</v>
+        <v>0.955</v>
       </c>
       <c r="J6" t="n">
-        <v>0.828</v>
+        <v>0.874</v>
       </c>
       <c r="K6" t="n">
-        <v>0.97</v>
+        <v>1.043</v>
       </c>
     </row>
     <row r="7">
@@ -695,28 +695,28 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.01</v>
+        <v>0.003</v>
       </c>
       <c r="E7" t="n">
         <v>0.002</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.034</v>
       </c>
       <c r="G7" t="n">
-        <v>0.007</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.013</v>
+        <v>0.006</v>
       </c>
       <c r="I7" t="n">
-        <v>1.01</v>
+        <v>1.003</v>
       </c>
       <c r="J7" t="n">
-        <v>1.007</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>1.014</v>
+        <v>1.006</v>
       </c>
     </row>
     <row r="8">
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2.435</v>
+        <v>2.436</v>
       </c>
       <c r="E8" t="n">
         <v>0.042</v>
@@ -746,16 +746,16 @@
         <v>2.353</v>
       </c>
       <c r="H8" t="n">
-        <v>2.517</v>
+        <v>2.519</v>
       </c>
       <c r="I8" t="n">
-        <v>11.421</v>
+        <v>11.431</v>
       </c>
       <c r="J8" t="n">
-        <v>10.522</v>
+        <v>10.521</v>
       </c>
       <c r="K8" t="n">
-        <v>12.397</v>
+        <v>12.421</v>
       </c>
     </row>
     <row r="9">
@@ -812,28 +812,28 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.121</v>
+        <v>0.122</v>
       </c>
       <c r="E10" t="n">
         <v>0.045</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0065</v>
+        <v>0.0069</v>
       </c>
       <c r="G10" t="n">
-        <v>0.034</v>
+        <v>0.033</v>
       </c>
       <c r="H10" t="n">
-        <v>0.209</v>
+        <v>0.21</v>
       </c>
       <c r="I10" t="n">
         <v>1.129</v>
       </c>
       <c r="J10" t="n">
-        <v>1.035</v>
+        <v>1.034</v>
       </c>
       <c r="K10" t="n">
-        <v>1.232</v>
+        <v>1.233</v>
       </c>
     </row>
     <row r="11">
@@ -890,28 +890,28 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-0.351</v>
+        <v>-0.316</v>
       </c>
       <c r="E12" t="n">
-        <v>0.056</v>
+        <v>0.054</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.46</v>
+        <v>-0.423</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.241</v>
+        <v>-0.209</v>
       </c>
       <c r="I12" t="n">
-        <v>0.704</v>
+        <v>0.729</v>
       </c>
       <c r="J12" t="n">
-        <v>0.631</v>
+        <v>0.655</v>
       </c>
       <c r="K12" t="n">
-        <v>0.786</v>
+        <v>0.8110000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -929,28 +929,28 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-0.006</v>
+        <v>-0.01</v>
       </c>
       <c r="E13" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.01</v>
+        <v>-0.013</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.003</v>
+        <v>-0.007</v>
       </c>
       <c r="I13" t="n">
-        <v>0.994</v>
+        <v>0.99</v>
       </c>
       <c r="J13" t="n">
-        <v>0.99</v>
+        <v>0.987</v>
       </c>
       <c r="K13" t="n">
-        <v>0.997</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="14">
@@ -977,19 +977,19 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>1.605</v>
+        <v>1.606</v>
       </c>
       <c r="H14" t="n">
-        <v>1.754</v>
+        <v>1.755</v>
       </c>
       <c r="I14" t="n">
-        <v>5.364</v>
+        <v>5.366</v>
       </c>
       <c r="J14" t="n">
-        <v>4.978</v>
+        <v>4.981</v>
       </c>
       <c r="K14" t="n">
-        <v>5.78</v>
+        <v>5.781</v>
       </c>
     </row>
     <row r="15">
@@ -1046,28 +1046,28 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>-0.035</v>
+        <v>-0.036</v>
       </c>
       <c r="E16" t="n">
         <v>0.094</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7126</v>
+        <v>0.7030999999999999</v>
       </c>
       <c r="G16" t="n">
         <v>-0.219</v>
       </c>
       <c r="H16" t="n">
-        <v>0.15</v>
+        <v>0.148</v>
       </c>
       <c r="I16" t="n">
-        <v>0.966</v>
+        <v>0.965</v>
       </c>
       <c r="J16" t="n">
         <v>0.803</v>
       </c>
       <c r="K16" t="n">
-        <v>1.161</v>
+        <v>1.159</v>
       </c>
     </row>
     <row r="17">
@@ -1091,7 +1091,7 @@
         <v>0.005</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0437</v>
+        <v>0.0443</v>
       </c>
       <c r="G17" t="n">
         <v>-0.021</v>
@@ -1100,7 +1100,7 @@
         <v>-0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.989</v>
+        <v>0.99</v>
       </c>
       <c r="J17" t="n">
         <v>0.979</v>
@@ -1124,28 +1124,28 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.258</v>
+        <v>-0.257</v>
       </c>
       <c r="E18" t="n">
-        <v>0.057</v>
+        <v>0.053</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.37</v>
+        <v>-0.361</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.146</v>
+        <v>-0.153</v>
       </c>
       <c r="I18" t="n">
-        <v>0.772</v>
+        <v>0.773</v>
       </c>
       <c r="J18" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.697</v>
       </c>
       <c r="K18" t="n">
-        <v>0.864</v>
+        <v>0.858</v>
       </c>
     </row>
     <row r="19">
@@ -1166,25 +1166,25 @@
         <v>-0.001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5803</v>
+        <v>0.4099</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.005</v>
+        <v>-0.004</v>
       </c>
       <c r="H19" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="I19" t="n">
         <v>0.999</v>
       </c>
       <c r="J19" t="n">
-        <v>0.995</v>
+        <v>0.996</v>
       </c>
       <c r="K19" t="n">
-        <v>1.003</v>
+        <v>1.001</v>
       </c>
     </row>
     <row r="20">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1.721</v>
+        <v>1.72</v>
       </c>
       <c r="E20" t="n">
         <v>0.022</v>
@@ -1211,19 +1211,19 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>1.678</v>
+        <v>1.677</v>
       </c>
       <c r="H20" t="n">
         <v>1.763</v>
       </c>
       <c r="I20" t="n">
-        <v>5.588</v>
+        <v>5.586</v>
       </c>
       <c r="J20" t="n">
-        <v>5.357</v>
+        <v>5.352</v>
       </c>
       <c r="K20" t="n">
-        <v>5.828</v>
+        <v>5.829</v>
       </c>
     </row>
     <row r="21">
@@ -1280,10 +1280,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.283</v>
+        <v>0.281</v>
       </c>
       <c r="E22" t="n">
-        <v>0.05</v>
+        <v>0.049</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1292,16 +1292,16 @@
         <v>0.185</v>
       </c>
       <c r="H22" t="n">
-        <v>0.381</v>
+        <v>0.377</v>
       </c>
       <c r="I22" t="n">
-        <v>1.327</v>
+        <v>1.324</v>
       </c>
       <c r="J22" t="n">
-        <v>1.204</v>
+        <v>1.203</v>
       </c>
       <c r="K22" t="n">
-        <v>1.463</v>
+        <v>1.458</v>
       </c>
     </row>
     <row r="23">
@@ -1358,28 +1358,28 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>-0.091</v>
+        <v>-0.062</v>
       </c>
       <c r="E24" t="n">
-        <v>0.056</v>
+        <v>0.057</v>
       </c>
       <c r="F24" t="n">
-        <v>0.104</v>
+        <v>0.2753</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.201</v>
+        <v>-0.173</v>
       </c>
       <c r="H24" t="n">
-        <v>0.019</v>
+        <v>0.049</v>
       </c>
       <c r="I24" t="n">
-        <v>0.913</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J24" t="n">
-        <v>0.8179999999999999</v>
+        <v>0.841</v>
       </c>
       <c r="K24" t="n">
-        <v>1.019</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="25">
@@ -1397,28 +1397,28 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>-0.003</v>
+        <v>-0.006</v>
       </c>
       <c r="E25" t="n">
         <v>0.002</v>
       </c>
       <c r="F25" t="n">
-        <v>0.07779999999999999</v>
+        <v>0.0002</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.006</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>-0.003</v>
       </c>
       <c r="I25" t="n">
+        <v>0.994</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.991</v>
+      </c>
+      <c r="K25" t="n">
         <v>0.997</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0.994</v>
-      </c>
-      <c r="K25" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1436,28 +1436,28 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2.365</v>
+        <v>2.367</v>
       </c>
       <c r="E26" t="n">
-        <v>0.04</v>
+        <v>0.041</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>2.286</v>
+        <v>2.287</v>
       </c>
       <c r="H26" t="n">
-        <v>2.444</v>
+        <v>2.447</v>
       </c>
       <c r="I26" t="n">
-        <v>10.641</v>
+        <v>10.662</v>
       </c>
       <c r="J26" t="n">
-        <v>9.832000000000001</v>
+        <v>9.840999999999999</v>
       </c>
       <c r="K26" t="n">
-        <v>11.517</v>
+        <v>11.551</v>
       </c>
     </row>
     <row r="27">
@@ -1514,28 +1514,28 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>-0.046</v>
+        <v>-0.044</v>
       </c>
       <c r="E28" t="n">
-        <v>0.074</v>
+        <v>0.075</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5319</v>
+        <v>0.5624</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.191</v>
+        <v>-0.192</v>
       </c>
       <c r="H28" t="n">
-        <v>0.099</v>
+        <v>0.104</v>
       </c>
       <c r="I28" t="n">
-        <v>0.955</v>
+        <v>0.957</v>
       </c>
       <c r="J28" t="n">
         <v>0.826</v>
       </c>
       <c r="K28" t="n">
-        <v>1.104</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="29">
@@ -1592,28 +1592,28 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>-0.53</v>
+        <v>-0.492</v>
       </c>
       <c r="E30" t="n">
-        <v>0.074</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.676</v>
+        <v>-0.632</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.384</v>
+        <v>-0.352</v>
       </c>
       <c r="I30" t="n">
-        <v>0.589</v>
+        <v>0.611</v>
       </c>
       <c r="J30" t="n">
-        <v>0.509</v>
+        <v>0.531</v>
       </c>
       <c r="K30" t="n">
-        <v>0.681</v>
+        <v>0.704</v>
       </c>
     </row>
     <row r="31">
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>-0.012</v>
+        <v>-0.016</v>
       </c>
       <c r="E31" t="n">
         <v>0.002</v>
@@ -1640,19 +1640,19 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.015</v>
+        <v>-0.019</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.008</v>
+        <v>-0.013</v>
       </c>
       <c r="I31" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="K31" t="n">
         <v>0.988</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0.985</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0.992</v>
       </c>
     </row>
     <row r="32">
@@ -1670,7 +1670,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>-1.349</v>
+        <v>-1.347</v>
       </c>
       <c r="E32" t="n">
         <v>0.064</v>
@@ -1679,10 +1679,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>-1.475</v>
+        <v>-1.473</v>
       </c>
       <c r="H32" t="n">
-        <v>-1.223</v>
+        <v>-1.221</v>
       </c>
       <c r="I32" t="n">
         <v>0.26</v>
@@ -1691,7 +1691,7 @@
         <v>0.229</v>
       </c>
       <c r="K32" t="n">
-        <v>0.294</v>
+        <v>0.295</v>
       </c>
     </row>
     <row r="33">
@@ -1748,28 +1748,28 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.372</v>
+        <v>0.376</v>
       </c>
       <c r="E34" t="n">
-        <v>0.094</v>
+        <v>0.097</v>
       </c>
       <c r="F34" t="n">
         <v>0.0001</v>
       </c>
       <c r="G34" t="n">
-        <v>0.188</v>
+        <v>0.187</v>
       </c>
       <c r="H34" t="n">
-        <v>0.555</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="I34" t="n">
-        <v>1.45</v>
+        <v>1.457</v>
       </c>
       <c r="J34" t="n">
-        <v>1.207</v>
+        <v>1.206</v>
       </c>
       <c r="K34" t="n">
-        <v>1.743</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="35">
@@ -1796,13 +1796,13 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.058</v>
+        <v>-0.059</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.037</v>
+        <v>-0.036</v>
       </c>
       <c r="I35" t="n">
-        <v>0.954</v>
+        <v>0.953</v>
       </c>
       <c r="J35" t="n">
         <v>0.9429999999999999</v>
@@ -1826,28 +1826,28 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>-0.746</v>
+        <v>-0.654</v>
       </c>
       <c r="E36" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.912</v>
+        <v>-0.825</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.579</v>
+        <v>-0.483</v>
       </c>
       <c r="I36" t="n">
-        <v>0.474</v>
+        <v>0.52</v>
       </c>
       <c r="J36" t="n">
-        <v>0.402</v>
+        <v>0.438</v>
       </c>
       <c r="K36" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.617</v>
       </c>
     </row>
     <row r="37">
@@ -1865,7 +1865,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>-0.017</v>
+        <v>-0.027</v>
       </c>
       <c r="E37" t="n">
         <v>0.002</v>
@@ -1874,19 +1874,19 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.02</v>
+        <v>-0.032</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.014</v>
+        <v>-0.022</v>
       </c>
       <c r="I37" t="n">
-        <v>0.983</v>
+        <v>0.973</v>
       </c>
       <c r="J37" t="n">
-        <v>0.98</v>
+        <v>0.969</v>
       </c>
       <c r="K37" t="n">
-        <v>0.986</v>
+        <v>0.978</v>
       </c>
     </row>
     <row r="38">
@@ -1907,16 +1907,16 @@
         <v>-0.338</v>
       </c>
       <c r="E38" t="n">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.397</v>
+        <v>-0.398</v>
       </c>
       <c r="H38" t="n">
-        <v>-0.28</v>
+        <v>-0.278</v>
       </c>
       <c r="I38" t="n">
         <v>0.713</v>
@@ -1925,7 +1925,7 @@
         <v>0.672</v>
       </c>
       <c r="K38" t="n">
-        <v>0.756</v>
+        <v>0.758</v>
       </c>
     </row>
     <row r="39">
@@ -1982,28 +1982,28 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>-0.289</v>
+        <v>-0.292</v>
       </c>
       <c r="E40" t="n">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.36</v>
+        <v>-0.364</v>
       </c>
       <c r="H40" t="n">
-        <v>-0.218</v>
+        <v>-0.22</v>
       </c>
       <c r="I40" t="n">
-        <v>0.749</v>
+        <v>0.747</v>
       </c>
       <c r="J40" t="n">
-        <v>0.698</v>
+        <v>0.695</v>
       </c>
       <c r="K40" t="n">
-        <v>0.804</v>
+        <v>0.803</v>
       </c>
     </row>
     <row r="41">
@@ -2027,7 +2027,7 @@
         <v>0.003</v>
       </c>
       <c r="F41" t="n">
-        <v>0.2114</v>
+        <v>0.1863</v>
       </c>
       <c r="G41" t="n">
         <v>-0.002</v>
@@ -2060,28 +2060,28 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>-0.202</v>
+        <v>-0.197</v>
       </c>
       <c r="E42" t="n">
-        <v>0.049</v>
+        <v>0.046</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.299</v>
+        <v>-0.286</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.105</v>
+        <v>-0.107</v>
       </c>
       <c r="I42" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.821</v>
       </c>
       <c r="J42" t="n">
-        <v>0.742</v>
+        <v>0.751</v>
       </c>
       <c r="K42" t="n">
-        <v>0.9</v>
+        <v>0.898</v>
       </c>
     </row>
     <row r="43">
@@ -2099,28 +2099,28 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E43" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.01</v>
+        <v>0.012</v>
       </c>
       <c r="H43" t="n">
-        <v>0.019</v>
+        <v>0.017</v>
       </c>
       <c r="I43" t="n">
-        <v>1.015</v>
+        <v>1.014</v>
       </c>
       <c r="J43" t="n">
-        <v>1.01</v>
+        <v>1.012</v>
       </c>
       <c r="K43" t="n">
-        <v>1.019</v>
+        <v>1.017</v>
       </c>
     </row>
     <row r="44">
@@ -2147,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.587</v>
+        <v>-0.586</v>
       </c>
       <c r="H44" t="n">
         <v>-0.452</v>
@@ -2156,7 +2156,7 @@
         <v>0.595</v>
       </c>
       <c r="J44" t="n">
-        <v>0.556</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="K44" t="n">
         <v>0.636</v>
@@ -2216,28 +2216,28 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>-0.819</v>
+        <v>-0.8149999999999999</v>
       </c>
       <c r="E46" t="n">
-        <v>0.144</v>
+        <v>0.143</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>-1.101</v>
+        <v>-1.096</v>
       </c>
       <c r="H46" t="n">
-        <v>-0.536</v>
+        <v>-0.534</v>
       </c>
       <c r="I46" t="n">
-        <v>0.441</v>
+        <v>0.443</v>
       </c>
       <c r="J46" t="n">
-        <v>0.332</v>
+        <v>0.334</v>
       </c>
       <c r="K46" t="n">
-        <v>0.585</v>
+        <v>0.586</v>
       </c>
     </row>
     <row r="47">
@@ -2294,28 +2294,28 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>-0.175</v>
+        <v>-0.137</v>
       </c>
       <c r="E48" t="n">
-        <v>0.066</v>
+        <v>0.064</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0076</v>
+        <v>0.031</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.304</v>
+        <v>-0.261</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.047</v>
+        <v>-0.012</v>
       </c>
       <c r="I48" t="n">
-        <v>0.839</v>
+        <v>0.872</v>
       </c>
       <c r="J48" t="n">
-        <v>0.738</v>
+        <v>0.77</v>
       </c>
       <c r="K48" t="n">
-        <v>0.955</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="49">
@@ -2333,7 +2333,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.011</v>
+        <v>0.008</v>
       </c>
       <c r="E49" t="n">
         <v>0.002</v>
@@ -2342,19 +2342,19 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0.007</v>
+        <v>0.004</v>
       </c>
       <c r="H49" t="n">
-        <v>0.016</v>
+        <v>0.011</v>
       </c>
       <c r="I49" t="n">
+        <v>1.008</v>
+      </c>
+      <c r="J49" t="n">
+        <v>1.004</v>
+      </c>
+      <c r="K49" t="n">
         <v>1.011</v>
-      </c>
-      <c r="J49" t="n">
-        <v>1.007</v>
-      </c>
-      <c r="K49" t="n">
-        <v>1.016</v>
       </c>
     </row>
     <row r="50">
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>-0.377</v>
+        <v>-0.376</v>
       </c>
       <c r="H52" t="n">
         <v>-0.204</v>
@@ -2492,10 +2492,10 @@
         <v>0.002</v>
       </c>
       <c r="E53" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="F53" t="n">
-        <v>0.519</v>
+        <v>0.5193</v>
       </c>
       <c r="G53" t="n">
         <v>-0.005</v>
@@ -2528,28 +2528,28 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>-0.331</v>
+        <v>-0.29</v>
       </c>
       <c r="E54" t="n">
-        <v>0.049</v>
+        <v>0.05</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>-0.428</v>
+        <v>-0.388</v>
       </c>
       <c r="H54" t="n">
-        <v>-0.234</v>
+        <v>-0.192</v>
       </c>
       <c r="I54" t="n">
-        <v>0.718</v>
+        <v>0.748</v>
       </c>
       <c r="J54" t="n">
-        <v>0.652</v>
+        <v>0.678</v>
       </c>
       <c r="K54" t="n">
-        <v>0.791</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="55">
@@ -2567,28 +2567,28 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.001</v>
+        <v>-0.003</v>
       </c>
       <c r="E55" t="n">
         <v>0.001</v>
       </c>
       <c r="F55" t="n">
-        <v>0.43</v>
+        <v>0.0196</v>
       </c>
       <c r="G55" t="n">
-        <v>-0.002</v>
+        <v>-0.006</v>
       </c>
       <c r="H55" t="n">
-        <v>0.004</v>
+        <v>-0.001</v>
       </c>
       <c r="I55" t="n">
-        <v>1.001</v>
+        <v>0.997</v>
       </c>
       <c r="J55" t="n">
-        <v>0.998</v>
+        <v>0.994</v>
       </c>
       <c r="K55" t="n">
-        <v>1.004</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="56">
@@ -2606,19 +2606,19 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>-2.674</v>
+        <v>-2.678</v>
       </c>
       <c r="E56" t="n">
-        <v>0.052</v>
+        <v>0.049</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>-2.776</v>
+        <v>-2.773</v>
       </c>
       <c r="H56" t="n">
-        <v>-2.573</v>
+        <v>-2.582</v>
       </c>
       <c r="I56" t="n">
         <v>0.06900000000000001</v>
@@ -2645,7 +2645,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.02</v>
+        <v>0.021</v>
       </c>
       <c r="E57" t="n">
         <v>0.001</v>
@@ -2666,7 +2666,7 @@
         <v>1.018</v>
       </c>
       <c r="K57" t="n">
-        <v>1.024</v>
+        <v>1.023</v>
       </c>
     </row>
     <row r="58">
@@ -2684,28 +2684,28 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.063</v>
       </c>
       <c r="E58" t="n">
-        <v>0.038</v>
+        <v>0.036</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0684</v>
+        <v>0.0788</v>
       </c>
       <c r="G58" t="n">
-        <v>-0.005</v>
+        <v>-0.007</v>
       </c>
       <c r="H58" t="n">
-        <v>0.144</v>
+        <v>0.132</v>
       </c>
       <c r="I58" t="n">
-        <v>1.072</v>
+        <v>1.065</v>
       </c>
       <c r="J58" t="n">
-        <v>0.995</v>
+        <v>0.993</v>
       </c>
       <c r="K58" t="n">
-        <v>1.155</v>
+        <v>1.141</v>
       </c>
     </row>
     <row r="59">
@@ -2723,16 +2723,16 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>-0.017</v>
+        <v>-0.016</v>
       </c>
       <c r="E59" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>-0.022</v>
+        <v>-0.021</v>
       </c>
       <c r="H59" t="n">
         <v>-0.012</v>
@@ -2762,28 +2762,28 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>-0.431</v>
+        <v>-0.459</v>
       </c>
       <c r="E60" t="n">
-        <v>0.076</v>
+        <v>0.065</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>-0.58</v>
+        <v>-0.586</v>
       </c>
       <c r="H60" t="n">
-        <v>-0.282</v>
+        <v>-0.332</v>
       </c>
       <c r="I60" t="n">
-        <v>0.65</v>
+        <v>0.632</v>
       </c>
       <c r="J60" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="K60" t="n">
-        <v>0.754</v>
+        <v>0.718</v>
       </c>
     </row>
     <row r="61">
@@ -2801,25 +2801,25 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>-0.008</v>
+        <v>-0.006</v>
       </c>
       <c r="E61" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0027</v>
+        <v>0.0009</v>
       </c>
       <c r="G61" t="n">
-        <v>-0.014</v>
+        <v>-0.01</v>
       </c>
       <c r="H61" t="n">
         <v>-0.003</v>
       </c>
       <c r="I61" t="n">
-        <v>0.992</v>
+        <v>0.994</v>
       </c>
       <c r="J61" t="n">
-        <v>0.987</v>
+        <v>0.99</v>
       </c>
       <c r="K61" t="n">
         <v>0.997</v>
@@ -2840,7 +2840,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>-0.768</v>
+        <v>-0.769</v>
       </c>
       <c r="E62" t="n">
         <v>0.02</v>
@@ -2852,7 +2852,7 @@
         <v>-0.8080000000000001</v>
       </c>
       <c r="H62" t="n">
-        <v>-0.728</v>
+        <v>-0.729</v>
       </c>
       <c r="I62" t="n">
         <v>0.464</v>
@@ -2861,7 +2861,7 @@
         <v>0.446</v>
       </c>
       <c r="K62" t="n">
-        <v>0.483</v>
+        <v>0.482</v>
       </c>
     </row>
     <row r="63">
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="H63" t="n">
         <v>0.012</v>
@@ -2918,7 +2918,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.381</v>
+        <v>0.38</v>
       </c>
       <c r="E64" t="n">
         <v>0.032</v>
@@ -2927,19 +2927,19 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0.319</v>
+        <v>0.317</v>
       </c>
       <c r="H64" t="n">
-        <v>0.444</v>
+        <v>0.443</v>
       </c>
       <c r="I64" t="n">
-        <v>1.464</v>
+        <v>1.463</v>
       </c>
       <c r="J64" t="n">
-        <v>1.375</v>
+        <v>1.374</v>
       </c>
       <c r="K64" t="n">
-        <v>1.558</v>
+        <v>1.557</v>
       </c>
     </row>
     <row r="65">
@@ -2996,28 +2996,28 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>-0.37</v>
+        <v>-0.351</v>
       </c>
       <c r="E66" t="n">
-        <v>0.033</v>
+        <v>0.032</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>-0.434</v>
+        <v>-0.414</v>
       </c>
       <c r="H66" t="n">
-        <v>-0.306</v>
+        <v>-0.287</v>
       </c>
       <c r="I66" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.704</v>
       </c>
       <c r="J66" t="n">
-        <v>0.648</v>
+        <v>0.661</v>
       </c>
       <c r="K66" t="n">
-        <v>0.737</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="67">
@@ -3035,7 +3035,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>-0.008999999999999999</v>
+        <v>-0.011</v>
       </c>
       <c r="E67" t="n">
         <v>0.001</v>
@@ -3044,19 +3044,19 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>-0.012</v>
+        <v>-0.013</v>
       </c>
       <c r="H67" t="n">
-        <v>-0.006</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="I67" t="n">
+        <v>0.989</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="K67" t="n">
         <v>0.991</v>
-      </c>
-      <c r="J67" t="n">
-        <v>0.989</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0.994</v>
       </c>
     </row>
     <row r="68">
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>1.298</v>
+        <v>1.299</v>
       </c>
       <c r="E68" t="n">
         <v>0.023</v>
@@ -3083,16 +3083,16 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>1.253</v>
+        <v>1.254</v>
       </c>
       <c r="H68" t="n">
         <v>1.344</v>
       </c>
       <c r="I68" t="n">
-        <v>3.663</v>
+        <v>3.665</v>
       </c>
       <c r="J68" t="n">
-        <v>3.5</v>
+        <v>3.503</v>
       </c>
       <c r="K68" t="n">
         <v>3.833</v>
@@ -3152,7 +3152,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.243</v>
+        <v>0.244</v>
       </c>
       <c r="E70" t="n">
         <v>0.048</v>
@@ -3164,16 +3164,16 @@
         <v>0.149</v>
       </c>
       <c r="H70" t="n">
-        <v>0.336</v>
+        <v>0.339</v>
       </c>
       <c r="I70" t="n">
-        <v>1.275</v>
+        <v>1.276</v>
       </c>
       <c r="J70" t="n">
-        <v>1.161</v>
+        <v>1.16</v>
       </c>
       <c r="K70" t="n">
-        <v>1.4</v>
+        <v>1.403</v>
       </c>
     </row>
     <row r="71">
@@ -3209,7 +3209,7 @@
         <v>0.981</v>
       </c>
       <c r="J71" t="n">
-        <v>0.976</v>
+        <v>0.975</v>
       </c>
       <c r="K71" t="n">
         <v>0.987</v>
@@ -3230,28 +3230,28 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>-0.169</v>
+        <v>-0.119</v>
       </c>
       <c r="E72" t="n">
-        <v>0.037</v>
+        <v>0.041</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>0.0038</v>
       </c>
       <c r="G72" t="n">
-        <v>-0.242</v>
+        <v>-0.2</v>
       </c>
       <c r="H72" t="n">
-        <v>-0.096</v>
+        <v>-0.039</v>
       </c>
       <c r="I72" t="n">
-        <v>0.845</v>
+        <v>0.888</v>
       </c>
       <c r="J72" t="n">
-        <v>0.785</v>
+        <v>0.819</v>
       </c>
       <c r="K72" t="n">
-        <v>0.908</v>
+        <v>0.962</v>
       </c>
     </row>
     <row r="73">
@@ -3269,28 +3269,28 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>-0.004</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="E73" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F73" t="n">
-        <v>0.0147</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>-0.007</v>
+        <v>-0.012</v>
       </c>
       <c r="H73" t="n">
-        <v>-0.001</v>
+        <v>-0.006</v>
       </c>
       <c r="I73" t="n">
-        <v>0.996</v>
+        <v>0.991</v>
       </c>
       <c r="J73" t="n">
-        <v>0.993</v>
+        <v>0.988</v>
       </c>
       <c r="K73" t="n">
-        <v>0.999</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="74">
@@ -3311,25 +3311,25 @@
         <v>1.459</v>
       </c>
       <c r="E74" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>1.43</v>
+        <v>1.431</v>
       </c>
       <c r="H74" t="n">
         <v>1.487</v>
       </c>
       <c r="I74" t="n">
-        <v>4.3</v>
+        <v>4.302</v>
       </c>
       <c r="J74" t="n">
-        <v>4.179</v>
+        <v>4.184</v>
       </c>
       <c r="K74" t="n">
-        <v>4.424</v>
+        <v>4.423</v>
       </c>
     </row>
     <row r="75">
@@ -3386,7 +3386,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.208</v>
+        <v>0.209</v>
       </c>
       <c r="E76" t="n">
         <v>0.05</v>
@@ -3395,19 +3395,19 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>0.111</v>
+        <v>0.11</v>
       </c>
       <c r="H76" t="n">
-        <v>0.305</v>
+        <v>0.308</v>
       </c>
       <c r="I76" t="n">
-        <v>1.231</v>
+        <v>1.232</v>
       </c>
       <c r="J76" t="n">
-        <v>1.117</v>
+        <v>1.116</v>
       </c>
       <c r="K76" t="n">
-        <v>1.357</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="77">
@@ -3425,7 +3425,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>-0.021</v>
+        <v>-0.022</v>
       </c>
       <c r="E77" t="n">
         <v>0.003</v>
@@ -3464,28 +3464,28 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>-0.27</v>
+        <v>-0.239</v>
       </c>
       <c r="E78" t="n">
-        <v>0.029</v>
+        <v>0.03</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>-0.327</v>
+        <v>-0.298</v>
       </c>
       <c r="H78" t="n">
-        <v>-0.213</v>
+        <v>-0.181</v>
       </c>
       <c r="I78" t="n">
-        <v>0.763</v>
+        <v>0.787</v>
       </c>
       <c r="J78" t="n">
-        <v>0.721</v>
+        <v>0.742</v>
       </c>
       <c r="K78" t="n">
-        <v>0.8080000000000001</v>
+        <v>0.835</v>
       </c>
     </row>
     <row r="79">
@@ -3503,7 +3503,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>-0.005</v>
+        <v>-0.008</v>
       </c>
       <c r="E79" t="n">
         <v>0.001</v>
@@ -3512,19 +3512,19 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="H79" t="n">
         <v>-0.007</v>
       </c>
-      <c r="H79" t="n">
-        <v>-0.003</v>
-      </c>
       <c r="I79" t="n">
-        <v>0.995</v>
+        <v>0.992</v>
       </c>
       <c r="J79" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="K79" t="n">
         <v>0.993</v>
-      </c>
-      <c r="K79" t="n">
-        <v>0.997</v>
       </c>
     </row>
     <row r="80">
@@ -3554,7 +3554,7 @@
         <v>-0.22</v>
       </c>
       <c r="H80" t="n">
-        <v>-0.068</v>
+        <v>-0.067</v>
       </c>
       <c r="I80" t="n">
         <v>0.866</v>
@@ -3620,28 +3620,28 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.091</v>
+        <v>0.09</v>
       </c>
       <c r="E82" t="n">
-        <v>0.061</v>
+        <v>0.06</v>
       </c>
       <c r="F82" t="n">
-        <v>0.1336</v>
+        <v>0.1355</v>
       </c>
       <c r="G82" t="n">
         <v>-0.028</v>
       </c>
       <c r="H82" t="n">
-        <v>0.21</v>
+        <v>0.209</v>
       </c>
       <c r="I82" t="n">
-        <v>1.095</v>
+        <v>1.094</v>
       </c>
       <c r="J82" t="n">
         <v>0.972</v>
       </c>
       <c r="K82" t="n">
-        <v>1.234</v>
+        <v>1.232</v>
       </c>
     </row>
     <row r="83">
@@ -3698,28 +3698,28 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>-0.446</v>
+        <v>-0.407</v>
       </c>
       <c r="E84" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>-0.572</v>
+        <v>-0.535</v>
       </c>
       <c r="H84" t="n">
-        <v>-0.32</v>
+        <v>-0.279</v>
       </c>
       <c r="I84" t="n">
-        <v>0.64</v>
+        <v>0.666</v>
       </c>
       <c r="J84" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.586</v>
       </c>
       <c r="K84" t="n">
-        <v>0.726</v>
+        <v>0.757</v>
       </c>
     </row>
     <row r="85">
@@ -3737,28 +3737,28 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>-0.005</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="E85" t="n">
         <v>0.002</v>
       </c>
       <c r="F85" t="n">
-        <v>0.006</v>
+        <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>-0.008999999999999999</v>
+        <v>-0.012</v>
       </c>
       <c r="H85" t="n">
-        <v>-0.001</v>
+        <v>-0.006</v>
       </c>
       <c r="I85" t="n">
-        <v>0.995</v>
+        <v>0.991</v>
       </c>
       <c r="J85" t="n">
-        <v>0.992</v>
+        <v>0.988</v>
       </c>
       <c r="K85" t="n">
-        <v>0.999</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="86">
@@ -3785,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>-0.531</v>
+        <v>-0.53</v>
       </c>
       <c r="H86" t="n">
         <v>-0.472</v>
@@ -3794,7 +3794,7 @@
         <v>0.606</v>
       </c>
       <c r="J86" t="n">
-        <v>0.588</v>
+        <v>0.589</v>
       </c>
       <c r="K86" t="n">
         <v>0.624</v>
@@ -3854,10 +3854,10 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.155</v>
+        <v>0.156</v>
       </c>
       <c r="E88" t="n">
-        <v>0.029</v>
+        <v>0.03</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -3866,16 +3866,16 @@
         <v>0.098</v>
       </c>
       <c r="H88" t="n">
-        <v>0.212</v>
+        <v>0.214</v>
       </c>
       <c r="I88" t="n">
-        <v>1.168</v>
+        <v>1.169</v>
       </c>
       <c r="J88" t="n">
         <v>1.103</v>
       </c>
       <c r="K88" t="n">
-        <v>1.236</v>
+        <v>1.239</v>
       </c>
     </row>
     <row r="89">
@@ -3911,7 +3911,7 @@
         <v>0.983</v>
       </c>
       <c r="J89" t="n">
-        <v>0.979</v>
+        <v>0.978</v>
       </c>
       <c r="K89" t="n">
         <v>0.987</v>
@@ -3932,28 +3932,28 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>-0.225</v>
+        <v>-0.188</v>
       </c>
       <c r="E90" t="n">
-        <v>0.034</v>
+        <v>0.036</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>-0.292</v>
+        <v>-0.259</v>
       </c>
       <c r="H90" t="n">
-        <v>-0.158</v>
+        <v>-0.118</v>
       </c>
       <c r="I90" t="n">
-        <v>0.798</v>
+        <v>0.828</v>
       </c>
       <c r="J90" t="n">
-        <v>0.747</v>
+        <v>0.772</v>
       </c>
       <c r="K90" t="n">
-        <v>0.854</v>
+        <v>0.889</v>
       </c>
     </row>
     <row r="91">
@@ -3971,7 +3971,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>-0.006</v>
+        <v>-0.01</v>
       </c>
       <c r="E91" t="n">
         <v>0.001</v>
@@ -3980,19 +3980,19 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>-0.008</v>
+        <v>-0.012</v>
       </c>
       <c r="H91" t="n">
-        <v>-0.003</v>
+        <v>-0.007</v>
       </c>
       <c r="I91" t="n">
-        <v>0.994</v>
+        <v>0.99</v>
       </c>
       <c r="J91" t="n">
-        <v>0.992</v>
+        <v>0.988</v>
       </c>
       <c r="K91" t="n">
-        <v>0.997</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="92">
@@ -4019,19 +4019,19 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>2.431</v>
+        <v>2.432</v>
       </c>
       <c r="H92" t="n">
         <v>2.494</v>
       </c>
       <c r="I92" t="n">
-        <v>11.734</v>
+        <v>11.739</v>
       </c>
       <c r="J92" t="n">
-        <v>11.374</v>
+        <v>11.378</v>
       </c>
       <c r="K92" t="n">
-        <v>12.106</v>
+        <v>12.112</v>
       </c>
     </row>
     <row r="93">
@@ -4088,28 +4088,28 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.161</v>
+        <v>0.162</v>
       </c>
       <c r="E94" t="n">
-        <v>0.042</v>
+        <v>0.043</v>
       </c>
       <c r="F94" t="n">
-        <v>0.0001</v>
+        <v>0.0002</v>
       </c>
       <c r="G94" t="n">
-        <v>0.079</v>
+        <v>0.078</v>
       </c>
       <c r="H94" t="n">
-        <v>0.244</v>
+        <v>0.246</v>
       </c>
       <c r="I94" t="n">
-        <v>1.175</v>
+        <v>1.176</v>
       </c>
       <c r="J94" t="n">
-        <v>1.082</v>
+        <v>1.081</v>
       </c>
       <c r="K94" t="n">
-        <v>1.276</v>
+        <v>1.278</v>
       </c>
     </row>
     <row r="95">
@@ -4148,7 +4148,7 @@
         <v>0.977</v>
       </c>
       <c r="K95" t="n">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="96">
@@ -4166,28 +4166,28 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>-0.224</v>
+        <v>-0.186</v>
       </c>
       <c r="E96" t="n">
-        <v>0.028</v>
+        <v>0.031</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>-0.28</v>
+        <v>-0.247</v>
       </c>
       <c r="H96" t="n">
-        <v>-0.169</v>
+        <v>-0.124</v>
       </c>
       <c r="I96" t="n">
-        <v>0.799</v>
+        <v>0.83</v>
       </c>
       <c r="J96" t="n">
-        <v>0.756</v>
+        <v>0.781</v>
       </c>
       <c r="K96" t="n">
-        <v>0.845</v>
+        <v>0.883</v>
       </c>
     </row>
     <row r="97">
@@ -4205,28 +4205,28 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>-0.001</v>
+        <v>-0.005</v>
       </c>
       <c r="E97" t="n">
         <v>0.001</v>
       </c>
       <c r="F97" t="n">
-        <v>0.2871</v>
+        <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>-0.004</v>
+        <v>-0.008</v>
       </c>
       <c r="H97" t="n">
-        <v>0.001</v>
+        <v>-0.003</v>
       </c>
       <c r="I97" t="n">
-        <v>0.999</v>
+        <v>0.995</v>
       </c>
       <c r="J97" t="n">
-        <v>0.996</v>
+        <v>0.992</v>
       </c>
       <c r="K97" t="n">
-        <v>1.001</v>
+        <v>0.997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>